<commit_message>
Completando el codigo 70 %
</commit_message>
<xml_diff>
--- a/predicciones.xlsx
+++ b/predicciones.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,120 +448,108 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Rechazada sin costas</t>
+          <t>Se declara admisible, 05 días. Dese cuenta ONI.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Admisibles</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Pide informe cumplimiento al fondo de la sentencia dentro de 08 días hábiles</t>
+          <t>Pone en conc.inhabilidad</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ica Solicita Diligencia</t>
+          <t>Acumulación</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dese cuenta</t>
+          <t>RESERVADO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dese Cuenta</t>
+          <t>Ica Informa</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ev. Informe. En relación</t>
+          <t>Dese cuenta admisibilidad</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Evacua Informe</t>
+          <t>Dese Cuenta</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Inicio tramitación</t>
+          <t>Incompetencia</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Inicio Tramitación</t>
+          <t>Incompetencia</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Agréguese Extraordinariamente a la tabla del 07 de febrero</t>
+          <t>Concede Recurso, Interconexión</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Agréguese A Tabla</t>
+          <t>Concede Apelación</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Pide informe cumplimiento de la sentencia de autos.</t>
+          <t>Dese cuenta en sala la apelación</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ica Solicita Diligencia</t>
+          <t>Dese Cuenta</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Prescinde informe, en relación</t>
+          <t>Ev. Informe. En relación.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Prescinde</t>
+          <t>Evacua Informe</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Habiéndose concedido a la recurrida ampliación de plazo para informar, el que a la fecha se encuentra vencido, pídase cuenta del informe solicitado en autos, debiendo evacuarlo dentro de tercero día, bajo apercibimiento de prescindir del mismo</t>
+          <t>Pide FUN dentro el palzo de 03 días</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Apercibe</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Dese Cuenta en Sala de Turno</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Dese Cuenta</t>
+          <t>Ica Solicita Diligencia</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregando mas datos a data agumentation
</commit_message>
<xml_diff>
--- a/predicciones.xlsx
+++ b/predicciones.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,156 +448,168 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>No ha lugar por extemporáneo la apelación de la recurrida</t>
+          <t>Ev. Informe. En relación</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ica Solicita Diligencia</t>
+          <t>Evacua Informe</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Deniega O.N.I.</t>
+          <t>Inadmisible</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Oni</t>
+          <t>Incompetencia</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ev. Informe.</t>
+          <t>Traslado</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Evacua Informe</t>
+          <t>Ica Informa</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Pide informar el domicilio contractual y el FUN actualizado del recurrente dentro de 05 días</t>
+          <t>Agréguese Extraordinariamente a la tabla del 03 de marzo</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ica Solicita Diligencia</t>
+          <t>Agréguese A Tabla</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Pide cuenta del informe a la recurrida</t>
+          <t>Ev. Informe. Pase al sr. presidente</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ica Solicita Diligencia</t>
+          <t>Evacua Informe</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Estese al mérito de autos</t>
+          <t>Se declara admisible, 05 días hábiles. Concede ONI.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ica Informa</t>
+          <t>Admisibles</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Inadmisible</t>
+          <t>Nota de Acuerdo: redacción Margarita Sanhueza</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Inadmisible/Omite</t>
+          <t>Acuerdo</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Concede Recurso, Interconexión</t>
+          <t>Concede ampliación de plazo por el término de 05 días</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Concede Apelación</t>
+          <t>Ica Amplia Plazo</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ev. Informe. En relación.</t>
+          <t>Concede ampliación de plazo por el término de 08 días</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Evacua Informe</t>
+          <t>Ica Amplia Plazo</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Comunica N° 14</t>
+          <t>Pide informe cumplimiento de sentencia a la recurrida</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ica Informa</t>
+          <t>Ica Solicita Diligencia</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dese Cuenta en Sala</t>
+          <t>Concede ampliación de Plazo por el término de 05 días</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Dese Cuenta</t>
+          <t>Ica Amplia Plazo</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Concede ampliación de plazo por el término de 05 días</t>
+          <t>No ha lugar ocúrrase ante quien corresponda</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ica Amplia Plazo</t>
+          <t>Ica Informa</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Se declara admisible, 08 días. Concede ONI.</t>
+          <t>Se declara admisible, 10 días. NHL ONI.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>Admisibles</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Concede recurso, interconexión</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Concede Apelación</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregando estructura al repositorio
</commit_message>
<xml_diff>
--- a/predicciones.xlsx
+++ b/predicciones.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ev. Informe. En relación</t>
+          <t>Ev. Informe. En Relación</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,31 +460,31 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Inadmisible</t>
+          <t>Estese al merito de autos</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Incompetencia</t>
+          <t>Ica Informa</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Traslado</t>
+          <t>Incompetencia</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ica Informa</t>
+          <t>Incompetencia</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Agréguese Extraordinariamente a la tabla del 03 de marzo</t>
+          <t>Agréguese Extraordinariamente a la tabla del 05 de marzo</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,19 +496,19 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ev. Informe. Pase al sr. presidente</t>
+          <t>Acogida sin costas</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Evacua Informe</t>
+          <t>Acoge</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Se declara admisible, 05 días hábiles. Concede ONI.</t>
+          <t>Acepta competencia: Se declara admisible, 10 días. NHL ONI.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,96 +520,168 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Nota de Acuerdo: redacción Margarita Sanhueza</t>
+          <t>Dese Cuenta en Sala de Turno</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Acuerdo</t>
+          <t>Dese Cuenta</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Concede ampliación de plazo por el término de 05 días</t>
+          <t>Agréguese Extraordinariamente</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ica Amplia Plazo</t>
+          <t>Agréguese A Tabla</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Concede ampliación de plazo por el término de 08 días</t>
+          <t>Al escrito tengase presente: Previo a resolver acompañese el documento ofrecido dentro del plazo de 05 días de tener por no presentado.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ica Amplia Plazo</t>
+          <t>Ica Solicita Diligencia</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Pide informe cumplimiento de sentencia a la recurrida</t>
+          <t>Inicio tramitación</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ica Solicita Diligencia</t>
+          <t>Inicio Tramitación</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Concede ampliación de Plazo por el término de 05 días</t>
+          <t>Nota de Acuerdo: Redacción Valentina Salvo Oviedo</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ica Amplia Plazo</t>
+          <t>Acuerdo</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>No ha lugar ocúrrase ante quien corresponda</t>
+          <t>Téngase Presente</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ica Informa</t>
+          <t>Téngase Presente</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Se declara admisible, 10 días. NHL ONI.</t>
+          <t>Dese cuenta admisibilidad</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Admisibles</t>
+          <t>Dese Cuenta</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Concede recurso, interconexión</t>
+          <t>Agréguese Extraordinariamente a la tabla del 07 de marzo</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Concede Apelación</t>
+          <t>Agréguese A Tabla</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Al folio 18: Téngase presente y como se pide.</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Téngase Presente</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Al folio 19: NHL. Al segundo otrosí, como se pide.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Nhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Téngase por reacusado</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Evacua Informe</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Agréguese Extraordinariamente a la tabla del 04 de marzo</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Agréguese A Tabla</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Téngase presente y por cumplido lo ordenado. En Relación</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Evacua Informe</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Rechazada sin costas</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Rechazada</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Modificando el archivo deploy
</commit_message>
<xml_diff>
--- a/predicciones.xlsx
+++ b/predicciones.xlsx
@@ -446,70 +446,70 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Rechazada sin costas</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rechazada</t>
+          <t>Ica Informa</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Se declara admisible 08 días. Concede ONI.</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Evacua Informe</t>
+          <t>Admisibles</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dese Cuenta Admisibilidad</t>
+          <t>Agréguese Extraordinariamente a la tabla del 05 de marzo</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dese Cuenta</t>
+          <t>Agréguese A Tabla</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ev. Informe. En relación</t>
+          <t>Rechazada sin costas</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Evacua Informe</t>
+          <t>Rechazada</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Inadmisible</t>
+          <t>Ev. Informe. En relación</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Incompetencia</t>
+          <t>Evacua Informe</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Agréguese Extraordinariamente a la tabla del 05 de marzo</t>
+          <t>Inadmisible</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Agréguese A Tabla</t>
+          <t>Inadmisible/Omite</t>
         </is>
       </c>
     </row>
@@ -528,48 +528,48 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Atendiendo al tiempo transcurrido y que la recurrida no ha evacuado el informe dese cuenta para los fines que diere lugar</t>
+          <t>Dese Cuenta Admisibilidad</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ica Solicita Diligencia</t>
+          <t>Dese Cuenta</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Concede ampliación de plazo por el término de 08 días hábiles</t>
+          <t>Se declara admisible, 10 días. Concede ONI.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ica Amplia Plazo</t>
+          <t>Admisibles</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Se declara admisible, 10 días. Concede ONI.</t>
+          <t>Concede ampliación de plazo por el término de 08 días hábiles</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Admisibles</t>
+          <t>Ica Amplia Plazo</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Se declara admisible 08 días. Concede ONI.</t>
+          <t>Atendiendo al tiempo transcurrido y que la recurrida no ha evacuado el informe dese cuenta para los fines que diere lugar</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Admisibles</t>
+          <t>Evacua Informe</t>
         </is>
       </c>
     </row>

</xml_diff>